<commit_message>
updated documentation and score reporting
</commit_message>
<xml_diff>
--- a/prep/AO/AO_ShoreAccess_output_JL20180126.xlsx
+++ b/prep/AO/AO_ShoreAccess_output_JL20180126.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-29800" yWindow="-2420" windowWidth="17800" windowHeight="11560"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17800" windowHeight="11560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ShorelineAccess_MHI" sheetId="4" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
-    <sheet name="ShoreAccess_output_Final_Calcs" sheetId="1" r:id="rId3"/>
-    <sheet name="Pivot" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="ShoreAccess_output_Final_Calcs" sheetId="1" r:id="rId4"/>
+    <sheet name="Pivot" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="65">
   <si>
     <t>MHI_reg</t>
   </si>
@@ -244,6 +245,24 @@
   </si>
   <si>
     <t>rgn_id</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High accessibility coastline </t>
+  </si>
+  <si>
+    <t>Moderate accessibility coastline with flat to moderate slopes near unpaved roads</t>
+  </si>
+  <si>
+    <t>Low accessibility coastlines with flat to moderate slopes near private roads or with no nearby road access</t>
+  </si>
+  <si>
+    <t>No access coastlines with cliffs or steep shorlines, no-take marine protected areas, and military areas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
   </si>
 </sst>
 </file>
@@ -636,6 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -666,7 +686,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1568,7 +1587,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" showMemberPropertyTips="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" showMemberPropertyTips="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
@@ -2012,7 +2031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:M6"/>
     </sheetView>
   </sheetViews>
@@ -2030,25 +2049,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="41" t="s">
+      <c r="E1" s="45"/>
+      <c r="F1" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="43" t="s">
+      <c r="G1" s="46"/>
+      <c r="H1" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="44"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="45"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="27" t="s">
@@ -2129,7 +2148,7 @@
         <f>I3*$I$2+J3*$J$2+K3</f>
         <v>0.6371437651532279</v>
       </c>
-      <c r="M3" s="51">
+      <c r="M3" s="41">
         <v>1</v>
       </c>
     </row>
@@ -2169,7 +2188,7 @@
         <f t="shared" ref="L4:L6" si="0">I4*$I$2+J4*$J$2+K4</f>
         <v>0.56026069720526683</v>
       </c>
-      <c r="M4" s="51">
+      <c r="M4" s="41">
         <v>4</v>
       </c>
     </row>
@@ -2211,7 +2230,7 @@
         <f t="shared" si="0"/>
         <v>0.55842896953401366</v>
       </c>
-      <c r="M5" s="51">
+      <c r="M5" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2253,7 +2272,7 @@
         <f t="shared" si="0"/>
         <v>0.67770866406366526</v>
       </c>
-      <c r="M6" s="51">
+      <c r="M6" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2276,8 +2295,8 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2287,22 +2306,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="3" spans="1:2" ht="144" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="49"/>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="49"/>
+      <c r="B5" s="50"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
@@ -2345,10 +2364,10 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="49"/>
+      <c r="B13" s="50"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
@@ -2387,6 +2406,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="143" x14ac:dyDescent="0.15">
+      <c r="A1" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B6">
+        <v>0.75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4779,7 +4861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E8"/>
   <sheetViews>

</xml_diff>